<commit_message>
Renamed and reorganized files
</commit_message>
<xml_diff>
--- a/utils/commit_counts.xlsx
+++ b/utils/commit_counts.xlsx
@@ -28,34 +28,34 @@
     <t>Group 1</t>
   </si>
   <si>
-    <t>LeeYinWei : 9</t>
-  </si>
-  <si>
-    <t>unknown899 : 16</t>
+    <t>LeeYinWei : 0</t>
+  </si>
+  <si>
+    <t>unknown899 : 0</t>
   </si>
   <si>
     <t>Group 2</t>
   </si>
   <si>
-    <t>neoAurora : 2</t>
+    <t>neoAurora : 0</t>
   </si>
   <si>
     <t>Lawrence16428 : 0</t>
   </si>
   <si>
-    <t>howardhung14 : 7</t>
+    <t>howardhung14 : 0</t>
   </si>
   <si>
     <t>Group 3</t>
   </si>
   <si>
-    <t>yoyo0213 : 19</t>
-  </si>
-  <si>
-    <t>JonathanYangSW : 21</t>
-  </si>
-  <si>
-    <t>GinoChen113511247 : 8</t>
+    <t>yoyo0213 : 0</t>
+  </si>
+  <si>
+    <t>JonathanYangSW : 0</t>
+  </si>
+  <si>
+    <t>GinoChen113511247 : 0</t>
   </si>
   <si>
     <t>Group 4</t>
@@ -64,49 +64,49 @@
     <t>JumboZhang1119 : 0</t>
   </si>
   <si>
-    <t>peienwu1216 : 32</t>
-  </si>
-  <si>
-    <t>chxyuuu : 5</t>
+    <t>peienwu1216 : 0</t>
+  </si>
+  <si>
+    <t>chxyuuu : 0</t>
   </si>
   <si>
     <t>Group 5</t>
   </si>
   <si>
-    <t>ginny923 : 4</t>
-  </si>
-  <si>
-    <t>joanna0420 : 1</t>
-  </si>
-  <si>
-    <t>dua0505 : 1</t>
+    <t>ginny923 : 0</t>
+  </si>
+  <si>
+    <t>joanna0420 : 0</t>
+  </si>
+  <si>
+    <t>dua0505 : 0</t>
   </si>
   <si>
     <t>Group 6</t>
   </si>
   <si>
-    <t>jui-pixel : 58</t>
+    <t>jui-pixel : 0</t>
   </si>
   <si>
     <t>SamTung113511034 : 0</t>
   </si>
   <si>
-    <t>charles691 : 8</t>
+    <t>charles691 : 0</t>
   </si>
   <si>
     <t>Group 7</t>
   </si>
   <si>
-    <t>Tony104147 : 12</t>
+    <t>Tony104147 : 0</t>
   </si>
   <si>
     <t>Group 8</t>
   </si>
   <si>
-    <t>haleychang0530 : 10</t>
-  </si>
-  <si>
-    <t>Hazel-1212 : 15</t>
+    <t>haleychang0530 : 0</t>
+  </si>
+  <si>
+    <t>Hazel-1212 : 0</t>
   </si>
   <si>
     <t>tree1014 : 0</t>
@@ -115,22 +115,22 @@
     <t>Group 9</t>
   </si>
   <si>
-    <t>CHENG-JE : 9</t>
-  </si>
-  <si>
-    <t>lwc-ed : 16</t>
+    <t>CHENG-JE : 0</t>
+  </si>
+  <si>
+    <t>lwc-ed : 0</t>
   </si>
   <si>
     <t>Group 10</t>
   </si>
   <si>
-    <t>tpvupu : 32</t>
-  </si>
-  <si>
-    <t>xiaotin22 : 53</t>
-  </si>
-  <si>
-    <t>calistayang : 11</t>
+    <t>tpvupu : 0</t>
+  </si>
+  <si>
+    <t>xiaotin22 : 0</t>
+  </si>
+  <si>
+    <t>calistayang : 0</t>
   </si>
   <si>
     <t>Group 11</t>
@@ -148,13 +148,13 @@
     <t>Group 12</t>
   </si>
   <si>
-    <t>kufanghua : 25</t>
-  </si>
-  <si>
-    <t>yezh0915 : 6</t>
-  </si>
-  <si>
-    <t>fiesta0217 : 6</t>
+    <t>kufanghua : 0</t>
+  </si>
+  <si>
+    <t>yezh0915 : 0</t>
+  </si>
+  <si>
+    <t>fiesta0217 : 0</t>
   </si>
   <si>
     <t>Group 13</t>
@@ -166,13 +166,13 @@
     <t>carabapy : 0</t>
   </si>
   <si>
-    <t>jing1688 : 59</t>
+    <t>jing1688 : 0</t>
   </si>
   <si>
     <t>Group 14</t>
   </si>
   <si>
-    <t>weiouo-0817 : 23</t>
+    <t>weiouo-0817 : 0</t>
   </si>
   <si>
     <t>NiNialpaca : 0</t>
@@ -181,31 +181,31 @@
     <t>Group 15</t>
   </si>
   <si>
-    <t>gamemode0701 : 11</t>
-  </si>
-  <si>
-    <t>Tonyyu2403 : 21</t>
+    <t>gamemode0701 : 0</t>
+  </si>
+  <si>
+    <t>Tonyyu2403 : 0</t>
   </si>
   <si>
     <t>Group 16</t>
   </si>
   <si>
-    <t>TerryCheese : 1</t>
-  </si>
-  <si>
-    <t>junlin27 : 6</t>
+    <t>TerryCheese : 0</t>
+  </si>
+  <si>
+    <t>junlin27 : 0</t>
   </si>
   <si>
     <t>Group 17</t>
   </si>
   <si>
-    <t>Miiaow3011 : 19</t>
-  </si>
-  <si>
-    <t>bonnieliao774 : 6</t>
-  </si>
-  <si>
-    <t>emmazheng0318 : 3</t>
+    <t>Miiaow3011 : 0</t>
+  </si>
+  <si>
+    <t>bonnieliao774 : 0</t>
+  </si>
+  <si>
+    <t>emmazheng0318 : 0</t>
   </si>
   <si>
     <t>Group 18</t>
@@ -214,7 +214,7 @@
     <t>ChocomintTW : 0</t>
   </si>
   <si>
-    <t>TedChueh : 3</t>
+    <t>TedChueh : 0</t>
   </si>
   <si>
     <t>pitinghsu : 0</t>
@@ -223,7 +223,7 @@
     <t>Group 19</t>
   </si>
   <si>
-    <t>max052028 : 1</t>
+    <t>max052028 : 0</t>
   </si>
   <si>
     <t>113511080 : 0</t>
@@ -232,13 +232,13 @@
     <t>Group 20</t>
   </si>
   <si>
-    <t>houyuankai : 4</t>
+    <t>houyuankai : 0</t>
   </si>
   <si>
     <t>Group 21</t>
   </si>
   <si>
-    <t>0u88 : 10</t>
+    <t>0u88 : 0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
chore: update workflow paths and README table structure
Updated GitHub Actions workflow to use utils directory for storing
pytest_results.txt and commit_counts.xlsx. Enhanced README table
structure to include detailed group information with commit counts
and statuses. Adjusted scripts to reflect updated file paths.
</commit_message>
<xml_diff>
--- a/utils/commit_counts.xlsx
+++ b/utils/commit_counts.xlsx
@@ -28,34 +28,34 @@
     <t>Group 1</t>
   </si>
   <si>
-    <t>LeeYinWei : 9</t>
-  </si>
-  <si>
-    <t>unknown899 : 16</t>
+    <t>LeeYinWei : 0</t>
+  </si>
+  <si>
+    <t>unknown899 : 0</t>
   </si>
   <si>
     <t>Group 2</t>
   </si>
   <si>
-    <t>neoAurora : 2</t>
+    <t>neoAurora : 0</t>
   </si>
   <si>
     <t>Lawrence16428 : 0</t>
   </si>
   <si>
-    <t>howardhung14 : 7</t>
+    <t>howardhung14 : 0</t>
   </si>
   <si>
     <t>Group 3</t>
   </si>
   <si>
-    <t>yoyo0213 : 19</t>
-  </si>
-  <si>
-    <t>JonathanYangSW : 21</t>
-  </si>
-  <si>
-    <t>GinoChen113511247 : 8</t>
+    <t>yoyo0213 : 0</t>
+  </si>
+  <si>
+    <t>JonathanYangSW : 0</t>
+  </si>
+  <si>
+    <t>GinoChen113511247 : 0</t>
   </si>
   <si>
     <t>Group 4</t>
@@ -64,49 +64,49 @@
     <t>JumboZhang1119 : 0</t>
   </si>
   <si>
-    <t>peienwu1216 : 32</t>
-  </si>
-  <si>
-    <t>chxyuuu : 5</t>
+    <t>peienwu1216 : 0</t>
+  </si>
+  <si>
+    <t>chxyuuu : 0</t>
   </si>
   <si>
     <t>Group 5</t>
   </si>
   <si>
-    <t>ginny923 : 4</t>
-  </si>
-  <si>
-    <t>joanna0420 : 1</t>
-  </si>
-  <si>
-    <t>dua0505 : 1</t>
+    <t>ginny923 : 0</t>
+  </si>
+  <si>
+    <t>joanna0420 : 0</t>
+  </si>
+  <si>
+    <t>dua0505 : 0</t>
   </si>
   <si>
     <t>Group 6</t>
   </si>
   <si>
-    <t>jui-pixel : 58</t>
+    <t>jui-pixel : 0</t>
   </si>
   <si>
     <t>SamTung113511034 : 0</t>
   </si>
   <si>
-    <t>charles691 : 8</t>
+    <t>charles691 : 0</t>
   </si>
   <si>
     <t>Group 7</t>
   </si>
   <si>
-    <t>Tony104147 : 12</t>
+    <t>Tony104147 : 0</t>
   </si>
   <si>
     <t>Group 8</t>
   </si>
   <si>
-    <t>haleychang0530 : 10</t>
-  </si>
-  <si>
-    <t>Hazel-1212 : 15</t>
+    <t>haleychang0530 : 0</t>
+  </si>
+  <si>
+    <t>Hazel-1212 : 0</t>
   </si>
   <si>
     <t>tree1014 : 0</t>
@@ -115,22 +115,22 @@
     <t>Group 9</t>
   </si>
   <si>
-    <t>CHENG-JE : 9</t>
-  </si>
-  <si>
-    <t>lwc-ed : 16</t>
+    <t>CHENG-JE : 0</t>
+  </si>
+  <si>
+    <t>lwc-ed : 0</t>
   </si>
   <si>
     <t>Group 10</t>
   </si>
   <si>
-    <t>tpvupu : 32</t>
-  </si>
-  <si>
-    <t>xiaotin22 : 53</t>
-  </si>
-  <si>
-    <t>calistayang : 11</t>
+    <t>tpvupu : 0</t>
+  </si>
+  <si>
+    <t>xiaotin22 : 0</t>
+  </si>
+  <si>
+    <t>calistayang : 0</t>
   </si>
   <si>
     <t>Group 11</t>
@@ -148,13 +148,13 @@
     <t>Group 12</t>
   </si>
   <si>
-    <t>kufanghua : 25</t>
-  </si>
-  <si>
-    <t>yezh0915 : 6</t>
-  </si>
-  <si>
-    <t>fiesta0217 : 6</t>
+    <t>kufanghua : 0</t>
+  </si>
+  <si>
+    <t>yezh0915 : 0</t>
+  </si>
+  <si>
+    <t>fiesta0217 : 0</t>
   </si>
   <si>
     <t>Group 13</t>
@@ -166,13 +166,13 @@
     <t>carabapy : 0</t>
   </si>
   <si>
-    <t>jing1688 : 59</t>
+    <t>jing1688 : 0</t>
   </si>
   <si>
     <t>Group 14</t>
   </si>
   <si>
-    <t>weiouo-0817 : 23</t>
+    <t>weiouo-0817 : 0</t>
   </si>
   <si>
     <t>NiNialpaca : 0</t>
@@ -181,31 +181,31 @@
     <t>Group 15</t>
   </si>
   <si>
-    <t>gamemode0701 : 11</t>
-  </si>
-  <si>
-    <t>Tonyyu2403 : 21</t>
+    <t>gamemode0701 : 0</t>
+  </si>
+  <si>
+    <t>Tonyyu2403 : 0</t>
   </si>
   <si>
     <t>Group 16</t>
   </si>
   <si>
-    <t>TerryCheese : 1</t>
-  </si>
-  <si>
-    <t>junlin27 : 6</t>
+    <t>TerryCheese : 0</t>
+  </si>
+  <si>
+    <t>junlin27 : 0</t>
   </si>
   <si>
     <t>Group 17</t>
   </si>
   <si>
-    <t>Miiaow3011 : 19</t>
-  </si>
-  <si>
-    <t>bonnieliao774 : 6</t>
-  </si>
-  <si>
-    <t>emmazheng0318 : 3</t>
+    <t>Miiaow3011 : 0</t>
+  </si>
+  <si>
+    <t>bonnieliao774 : 0</t>
+  </si>
+  <si>
+    <t>emmazheng0318 : 0</t>
   </si>
   <si>
     <t>Group 18</t>
@@ -214,7 +214,7 @@
     <t>ChocomintTW : 0</t>
   </si>
   <si>
-    <t>TedChueh : 3</t>
+    <t>TedChueh : 0</t>
   </si>
   <si>
     <t>pitinghsu : 0</t>
@@ -223,7 +223,7 @@
     <t>Group 19</t>
   </si>
   <si>
-    <t>max052028 : 1</t>
+    <t>max052028 : 0</t>
   </si>
   <si>
     <t>113511080 : 0</t>
@@ -232,13 +232,13 @@
     <t>Group 20</t>
   </si>
   <si>
-    <t>houyuankai : 4</t>
+    <t>houyuankai : 0</t>
   </si>
   <si>
     <t>Group 21</t>
   </si>
   <si>
-    <t>0u88 : 10</t>
+    <t>0u88 : 0</t>
   </si>
 </sst>
 </file>

</xml_diff>